<commit_message>
LR 3(1) the second turn
</commit_message>
<xml_diff>
--- a/LR3/table_1_36.xlsx
+++ b/LR3/table_1_36.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saida\Desktop\Учеба\ИТ Алекссев\ЛР 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B03E37-D050-4F6E-9A02-C40B3590AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109868D1-4101-48AC-BE35-6FA64BA46BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>№ квартиры</t>
   </si>
   <si>
-    <t>Фамилия квартиросъемщика</t>
-  </si>
-  <si>
     <t>Сумма, руб.</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>Просрочка, дней</t>
+  </si>
+  <si>
+    <t>Фамилия квартиросъёмщика</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,34 +572,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <f>C3-0.5</f>
@@ -693,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="5"/>
@@ -783,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="5"/>
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="5"/>
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="5"/>
@@ -918,7 +918,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="5"/>
@@ -963,7 +963,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="5"/>
@@ -1008,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="5"/>
@@ -1053,7 +1053,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="5"/>
@@ -1098,7 +1098,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="5"/>
@@ -1143,7 +1143,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="5"/>
@@ -1188,7 +1188,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="5"/>
@@ -1233,7 +1233,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="5"/>
@@ -1278,7 +1278,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="5"/>
@@ -1323,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="5"/>
@@ -1368,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="5"/>
@@ -1413,7 +1413,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="5"/>
@@ -1458,7 +1458,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="5"/>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="5"/>
@@ -1548,7 +1548,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="5"/>
@@ -1593,7 +1593,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="5"/>
@@ -1638,7 +1638,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="5"/>
@@ -1683,7 +1683,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="5"/>
@@ -1728,7 +1728,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="5"/>
@@ -1773,7 +1773,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="5"/>
@@ -1818,7 +1818,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="5"/>
@@ -1863,7 +1863,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="5"/>
@@ -1908,7 +1908,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="5"/>
@@ -1953,7 +1953,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="5"/>
@@ -1998,7 +1998,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="5"/>
@@ -2043,7 +2043,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="5"/>
@@ -2088,7 +2088,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="5"/>
@@ -2133,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="5"/>
@@ -2178,7 +2178,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="5"/>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="40" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <f>FLOOR(SUM(K3:K38), 1)</f>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="41" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <f>AVERAGE(C3:C38)</f>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <f>MAX(H3:H38)</f>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="43" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
LR 3(1) the third turn
</commit_message>
<xml_diff>
--- a/LR3/table_1_36.xlsx
+++ b/LR3/table_1_36.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109868D1-4101-48AC-BE35-6FA64BA46BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C448FC70-C31C-4287-91EF-4696FDBAFD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,18 +68,12 @@
     <t>Асадуллин</t>
   </si>
   <si>
-    <t xml:space="preserve">Афанасьев </t>
-  </si>
-  <si>
     <t>Бикмухаметов</t>
   </si>
   <si>
     <t>Боровик</t>
   </si>
   <si>
-    <t xml:space="preserve">Галимов </t>
-  </si>
-  <si>
     <t>Гиниатулин</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>Шаабан</t>
   </si>
   <si>
-    <t xml:space="preserve">Шалаев </t>
-  </si>
-  <si>
     <t>Шарафан</t>
   </si>
   <si>
@@ -155,12 +146,6 @@
     <t>Куропаткин 1</t>
   </si>
   <si>
-    <t>Куропаткин 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Угурлуэл </t>
-  </si>
-  <si>
     <t>Банницин</t>
   </si>
   <si>
@@ -189,6 +174,21 @@
   </si>
   <si>
     <t>Фамилия квартиросъёмщика</t>
+  </si>
+  <si>
+    <t>Афанасьев</t>
+  </si>
+  <si>
+    <t>Галимов</t>
+  </si>
+  <si>
+    <t>Угурлуэл</t>
+  </si>
+  <si>
+    <t>Шалаев</t>
+  </si>
+  <si>
+    <t>Мохамед</t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -251,6 +251,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -534,13 +540,13 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.7265625" customWidth="1"/>
     <col min="4" max="4" width="17.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.7265625" customWidth="1"/>
@@ -556,7 +562,7 @@
       <c r="A1" s="1">
         <v>36</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -572,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -590,10 +596,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>5</v>
@@ -606,14 +612,14 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
       </c>
       <c r="D3" s="1">
-        <f>A1*1.1</f>
+        <f>$A$1*1.1</f>
         <v>39.6</v>
       </c>
       <c r="E3" s="1">
@@ -647,7 +653,7 @@
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1">
@@ -655,11 +661,11 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f>D3</f>
+        <f t="shared" ref="D4:D34" si="0">$A$1*1.1</f>
         <v>39.6</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E38" si="0">C4*D4</f>
+        <f t="shared" ref="E4:E38" si="1">C4*D4</f>
         <v>2752.2000000000003</v>
       </c>
       <c r="F4" s="5">
@@ -671,7 +677,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H38" si="1">IF(G4&gt;F4,G4-F4,0)</f>
+        <f t="shared" ref="H4:H38" si="2">IF(G4&gt;F4,G4-F4,0)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
@@ -679,32 +685,32 @@
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J38" si="2">H4*I4</f>
+        <f t="shared" ref="J4:J38" si="3">H4*I4</f>
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K38" si="3">E4+J4</f>
+        <f t="shared" ref="K4:K38" si="4">E4+J4</f>
         <v>2752.2000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <f t="shared" ref="A5:A38" si="4">A4+1</f>
+        <f t="shared" ref="A5:A38" si="5">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
+        <f t="shared" ref="C5:C38" si="6">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D34" si="6">D4</f>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2732.4</v>
       </c>
       <c r="F5" s="5">
@@ -716,7 +722,7 @@
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
@@ -724,32 +730,32 @@
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2732.4</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2712.6</v>
       </c>
       <c r="F6" s="5">
@@ -761,7 +767,7 @@
         <v>44808</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
@@ -769,32 +775,32 @@
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2712.6</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
+      <c r="B7" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2692.8</v>
       </c>
       <c r="F7" s="5">
@@ -806,7 +812,7 @@
         <v>44809</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
@@ -814,32 +820,32 @@
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2692.8</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2673</v>
       </c>
       <c r="F8" s="5">
@@ -851,7 +857,7 @@
         <v>44810</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
@@ -859,32 +865,32 @@
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2673</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2653.2000000000003</v>
       </c>
       <c r="F9" s="5">
@@ -896,7 +902,7 @@
         <v>44811</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -904,32 +910,32 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2653.2000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
+      <c r="B10" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2633.4</v>
       </c>
       <c r="F10" s="5">
@@ -941,7 +947,7 @@
         <v>44812</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
@@ -949,32 +955,32 @@
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2633.4</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2613.6</v>
       </c>
       <c r="F11" s="5">
@@ -986,7 +992,7 @@
         <v>44813</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11" s="1">
@@ -994,32 +1000,32 @@
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2613.6</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2593.8000000000002</v>
       </c>
       <c r="F12" s="5">
@@ -1031,7 +1037,7 @@
         <v>44814</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
@@ -1039,32 +1045,32 @@
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2603.8000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2574</v>
       </c>
       <c r="F13" s="5">
@@ -1076,7 +1082,7 @@
         <v>44815</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I13" s="1">
@@ -1084,32 +1090,32 @@
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2594</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
+      <c r="B14" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2554.2000000000003</v>
       </c>
       <c r="F14" s="5">
@@ -1121,7 +1127,7 @@
         <v>44816</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I14" s="1">
@@ -1129,32 +1135,32 @@
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2584.2000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
+      <c r="B15" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2534.4</v>
       </c>
       <c r="F15" s="5">
@@ -1166,7 +1172,7 @@
         <v>44817</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I15" s="1">
@@ -1174,32 +1180,32 @@
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2574.4</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2514.6</v>
       </c>
       <c r="F16" s="5">
@@ -1211,7 +1217,7 @@
         <v>44818</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I16" s="1">
@@ -1219,32 +1225,32 @@
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2564.6</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2494.8000000000002</v>
       </c>
       <c r="F17" s="5">
@@ -1256,7 +1262,7 @@
         <v>44819</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I17" s="1">
@@ -1264,32 +1270,32 @@
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2554.8000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
+      <c r="B18" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2475</v>
       </c>
       <c r="F18" s="5">
@@ -1301,7 +1307,7 @@
         <v>44820</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="I18" s="1">
@@ -1309,32 +1315,32 @@
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2545</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
+      <c r="B19" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2455.2000000000003</v>
       </c>
       <c r="F19" s="5">
@@ -1346,7 +1352,7 @@
         <v>44821</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I19" s="1">
@@ -1354,32 +1360,32 @@
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2535.2000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2435.4</v>
       </c>
       <c r="F20" s="5">
@@ -1391,7 +1397,7 @@
         <v>44822</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I20" s="1">
@@ -1399,32 +1405,32 @@
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2525.4</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
+      <c r="B21" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2415.6</v>
       </c>
       <c r="F21" s="5">
@@ -1436,7 +1442,7 @@
         <v>44823</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I21" s="1">
@@ -1444,32 +1450,32 @@
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2515.6</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
+      <c r="B22" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2395.8000000000002</v>
       </c>
       <c r="F22" s="5">
@@ -1481,7 +1487,7 @@
         <v>44824</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I22" s="1">
@@ -1489,32 +1495,32 @@
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2505.8000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
+      <c r="B23" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2376</v>
       </c>
       <c r="F23" s="5">
@@ -1526,7 +1532,7 @@
         <v>44825</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I23" s="1">
@@ -1534,32 +1540,32 @@
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2496</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>27</v>
+      <c r="B24" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2356.2000000000003</v>
       </c>
       <c r="F24" s="5">
@@ -1571,7 +1577,7 @@
         <v>44826</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I24" s="1">
@@ -1579,32 +1585,32 @@
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2486.2000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
+      <c r="B25" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2336.4</v>
       </c>
       <c r="F25" s="5">
@@ -1616,7 +1622,7 @@
         <v>44827</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="I25" s="1">
@@ -1624,32 +1630,32 @@
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2476.4</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>40</v>
+      <c r="B26" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2316.6</v>
       </c>
       <c r="F26" s="5">
@@ -1661,7 +1667,7 @@
         <v>44828</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I26" s="1">
@@ -1669,32 +1675,32 @@
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2466.6</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>29</v>
+      <c r="B27" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2296.8000000000002</v>
       </c>
       <c r="F27" s="5">
@@ -1706,7 +1712,7 @@
         <v>44829</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="I27" s="1">
@@ -1714,33 +1720,33 @@
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2456.8000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>30</v>
+      <c r="B28" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f>D3/3</f>
-        <v>13.200000000000001</v>
+        <f t="shared" si="0"/>
+        <v>39.6</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>759.00000000000011</v>
+        <f t="shared" si="1"/>
+        <v>2277</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="7"/>
@@ -1751,7 +1757,7 @@
         <v>44830</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="I28" s="1">
@@ -1759,32 +1765,32 @@
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="3"/>
-        <v>929.00000000000011</v>
+        <f t="shared" si="4"/>
+        <v>2447</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>31</v>
+      <c r="B29" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f>D3</f>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2257.2000000000003</v>
       </c>
       <c r="F29" s="5">
@@ -1796,7 +1802,7 @@
         <v>44831</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="I29" s="1">
@@ -1804,32 +1810,32 @@
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2437.2000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>32</v>
+      <c r="B30" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2237.4</v>
       </c>
       <c r="F30" s="5">
@@ -1841,7 +1847,7 @@
         <v>44832</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="I30" s="1">
@@ -1849,32 +1855,32 @@
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2427.4</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
+      <c r="B31" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2217.6</v>
       </c>
       <c r="F31" s="5">
@@ -1886,7 +1892,7 @@
         <v>44833</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="I31" s="1">
@@ -1894,32 +1900,32 @@
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2417.6</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
+      <c r="B32" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2197.8000000000002</v>
       </c>
       <c r="F32" s="5">
@@ -1931,7 +1937,7 @@
         <v>44834</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="I32" s="1">
@@ -1939,32 +1945,32 @@
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2407.8000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>35</v>
+      <c r="B33" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2178</v>
       </c>
       <c r="F33" s="5">
@@ -1976,7 +1982,7 @@
         <v>44835</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="I33" s="1">
@@ -1984,32 +1990,32 @@
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2398</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
+      <c r="B34" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>39.6</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2158.2000000000003</v>
       </c>
       <c r="F34" s="5">
@@ -2021,7 +2027,7 @@
         <v>44836</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="I34" s="1">
@@ -2029,33 +2035,33 @@
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>230</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2388.2000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
+      <c r="B35" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>D3/3</f>
-        <v>13.200000000000001</v>
+        <f>$A$1*1.1/2</f>
+        <v>19.8</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
-        <v>712.80000000000007</v>
+        <f t="shared" si="1"/>
+        <v>1069.2</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" si="7"/>
@@ -2066,7 +2072,7 @@
         <v>44837</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="I35" s="1">
@@ -2074,32 +2080,32 @@
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="3"/>
-        <v>952.80000000000007</v>
+        <f t="shared" si="4"/>
+        <v>1309.2</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>41</v>
+      <c r="B36" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f>D3/2</f>
+        <f t="shared" ref="D36:D38" si="10">$A$1*1.1/2</f>
         <v>19.8</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1059.3</v>
       </c>
       <c r="F36" s="5">
@@ -2111,7 +2117,7 @@
         <v>44838</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="I36" s="1">
@@ -2119,32 +2125,32 @@
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1309.3</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>38</v>
+      <c r="B37" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" ref="D37:D38" si="10">D4/2</f>
+        <f t="shared" si="10"/>
         <v>19.8</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1049.4000000000001</v>
       </c>
       <c r="F37" s="5">
@@ -2156,7 +2162,7 @@
         <v>44839</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="I37" s="1">
@@ -2164,24 +2170,24 @@
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1309.4000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>39</v>
+      <c r="B38" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
@@ -2189,7 +2195,7 @@
         <v>19.8</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1039.5</v>
       </c>
       <c r="F38" s="5">
@@ -2201,7 +2207,7 @@
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="I38" s="1">
@@ -2209,11 +2215,11 @@
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1309.5</v>
       </c>
     </row>
@@ -2221,17 +2227,17 @@
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="1" t="s">
-        <v>45</v>
+      <c r="B40" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="C40">
         <f>FLOOR(SUM(K3:K38), 1)</f>
-        <v>85006</v>
+        <v>86880</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
-        <v>46</v>
+      <c r="B41" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C41">
         <f>AVERAGE(C3:C38)</f>
@@ -2239,8 +2245,8 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
-        <v>47</v>
+      <c r="B42" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C42">
         <f>MAX(H3:H38)</f>
@@ -2248,8 +2254,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B43" s="1" t="s">
-        <v>48</v>
+      <c r="B43" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C43">
         <f>MAX(K3:K38)</f>

</xml_diff>

<commit_message>
LR 3 (1) the fourth turn
</commit_message>
<xml_diff>
--- a/LR3/table_1_36.xlsx
+++ b/LR3/table_1_36.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C448FC70-C31C-4287-91EF-4696FDBAFD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50C6299-417C-405E-8FA2-658056052A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2231,7 +2231,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <f>FLOOR(SUM(K3:K38), 1)</f>
+        <f>FLOOR(SUM(K3:K38),1)</f>
         <v>86880</v>
       </c>
     </row>

</xml_diff>